<commit_message>
added: file .csv and basic-auth
</commit_message>
<xml_diff>
--- a/Suma_Tiempos.xlsx
+++ b/Suma_Tiempos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Ñoño Barriga</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>Etapa 3</t>
+  </si>
+  <si>
+    <t>Etapa 4</t>
+  </si>
+  <si>
+    <t>Etapa 5</t>
+  </si>
+  <si>
+    <t>Etapa 6</t>
+  </si>
+  <si>
+    <t>Etapa 7</t>
   </si>
   <si>
     <t>Total</t>
@@ -75,6 +87,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -97,12 +110,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -193,10 +208,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -398,158 +413,230 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="n">
+        <v>0.0766782407407407</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="n">
+        <v>0.0718634259259259</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="n">
+        <v>0.0725578703703704</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="n">
+        <v>0.0760300925925926</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="n">
         <f aca="false">SUM(B3:B5)</f>
         <v>0.216666666666667</v>
       </c>
-      <c r="C6" s="6" t="n">
+      <c r="C10" s="6" t="n">
         <f aca="false">SUM(C3:C5)</f>
         <v>0.222222222222222</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D10" s="6" t="n">
         <f aca="false">SUM(D3:D5)</f>
         <v>0.207638888888889</v>
       </c>
-      <c r="E6" s="6" t="n">
-        <f aca="false">SUM(E3:E5)</f>
-        <v>0.205810185185185</v>
-      </c>
-      <c r="F6" s="6" t="n">
+      <c r="E10" s="6" t="n">
+        <f aca="false">SUM(E3:E9)</f>
+        <v>0.502939814814815</v>
+      </c>
+      <c r="F10" s="6" t="n">
         <f aca="false">SUM(F3:F5)</f>
         <v>0.209375</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G10" s="6" t="n">
         <f aca="false">SUM(G3:G5)</f>
         <v>0.196527777777778</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H10" s="6" t="n">
         <f aca="false">SUM(H3:H5)</f>
         <v>0.189583333333333</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I10" s="6" t="n">
         <f aca="false">SUM(I3:I5)</f>
         <v>0.186111111111111</v>
       </c>
-      <c r="J6" s="6" t="n">
+      <c r="J10" s="6" t="n">
         <f aca="false">SUM(J3:J5)</f>
         <v>0.186111111111111</v>
       </c>
-      <c r="K6" s="6" t="n">
+      <c r="K10" s="6" t="n">
         <f aca="false">SUM(K3:K5)</f>
         <v>0.183333333333333</v>
       </c>
-      <c r="L6" s="6" t="n">
+      <c r="L10" s="6" t="n">
         <f aca="false">SUM(L3:L5)</f>
         <v>0.179166666666667</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="n">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C13" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F13" s="0" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="4" t="n">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="4" t="n">
         <v>0.0381944444444444</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C15" s="4" t="n">
         <v>0.0402777777777778</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D15" s="4" t="n">
         <v>0.0347222222222222</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E15" s="4" t="n">
         <v>0.0375</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F15" s="4" t="n">
         <v>0.0370601851851852</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="4" t="n">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="4" t="n">
         <v>0.0972222222222222</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="C16" s="4" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D16" s="4" t="n">
         <v>0.0902777777777778</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E16" s="4" t="n">
         <v>0.0854166666666667</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F16" s="4" t="n">
         <v>0.0819444444444444</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="4" t="n">
         <v>0.0868055555555556</v>
       </c>
-      <c r="C13" s="4" t="n">
+      <c r="C17" s="4" t="n">
         <v>0.0930555555555556</v>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D17" s="4" t="n">
         <v>0.084375</v>
       </c>
-      <c r="E13" s="4" t="n">
+      <c r="E17" s="4" t="n">
         <v>0.0847222222222222</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F17" s="4" t="n">
         <v>0.0868055555555556</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6" t="n">
-        <f aca="false">SUM(B11:B13)</f>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6" t="n">
+        <f aca="false">SUM(B15:B17)</f>
         <v>0.222222222222222</v>
       </c>
-      <c r="C14" s="6" t="n">
-        <f aca="false">SUM(C11:C13)</f>
+      <c r="C18" s="6" t="n">
+        <f aca="false">SUM(C15:C17)</f>
         <v>0.216666666666667</v>
       </c>
-      <c r="D14" s="6" t="n">
-        <f aca="false">SUM(D11:D13)</f>
+      <c r="D18" s="6" t="n">
+        <f aca="false">SUM(D15:D17)</f>
         <v>0.209375</v>
       </c>
-      <c r="E14" s="6" t="n">
-        <f aca="false">SUM(E11:E13)</f>
+      <c r="E18" s="6" t="n">
+        <f aca="false">SUM(E15:E17)</f>
         <v>0.207638888888889</v>
       </c>
-      <c r="F14" s="6" t="n">
-        <f aca="false">SUM(F11:F13)</f>
+      <c r="F18" s="6" t="n">
+        <f aca="false">SUM(F15:F17)</f>
         <v>0.205810185185185</v>
       </c>
     </row>

</xml_diff>